<commit_message>
Day updates. Graphing autorange and graph range options working
</commit_message>
<xml_diff>
--- a/grid window layouts.xlsx
+++ b/grid window layouts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndwebb\git\MatPlotLim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6434A4B-20DD-487D-A1F8-8583630897F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2F0437-4B4D-4DA7-9D4F-C510C9C8927F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FBD1CDCF-63DC-4640-A7CB-BA4E3AB49651}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{FBD1CDCF-63DC-4640-A7CB-BA4E3AB49651}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data_w" sheetId="1" r:id="rId1"/>
+    <sheet name="graph_w" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,9 +33,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Data Description</t>
+  </si>
+  <si>
+    <t>Text_desc_w</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>TextBox</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Filter Data</t>
+  </si>
+  <si>
+    <t>Filt Col</t>
+  </si>
+  <si>
+    <t>Filt Term</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Remove Data</t>
+  </si>
+  <si>
+    <t>Add Selected Group</t>
+  </si>
+  <si>
+    <t>Invert?</t>
+  </si>
+  <si>
+    <t>Color_dropdown</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +114,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -59,12 +162,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,14 +560,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4EF3D0-69DA-464F-97FB-5889A7523E93}">
-  <dimension ref="A1"/>
+  <dimension ref="D2:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="11"/>
+      <c r="P5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:I5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C639AA71-47D4-4CB9-B735-8A54AF530487}">
+  <dimension ref="C3:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="11"/>
+      <c r="O6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="13"/>
+      <c r="O7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F6:H6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>